<commit_message>
Adds UX 1 and UX 2 results
</commit_message>
<xml_diff>
--- a/docs/user study/results/UX 1.xlsx
+++ b/docs/user study/results/UX 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varma\Documents\GitHub\MSAT-UI\docs\user study\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD42F40-ABB6-46EE-B7A6-B159A06E3DC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB38470-71CE-4C44-9F79-731488D5CEF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16110" yWindow="1110" windowWidth="8715" windowHeight="6090" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,25 @@
     <sheet name="RQ 2" sheetId="3" r:id="rId3"/>
     <sheet name="RQ 3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="53">
   <si>
     <t xml:space="preserve">How often do you do software development? </t>
   </si>
@@ -126,9 +134,6 @@
     <t>Prototype 2 [ Separate List ]</t>
   </si>
   <si>
-    <t>Prototype 3 [ StackOverFlow UI ]</t>
-  </si>
-  <si>
     <t>Icon rotation / animation</t>
   </si>
   <si>
@@ -184,6 +189,12 @@
   </si>
   <si>
     <t>Special attention is needed for UI.</t>
+  </si>
+  <si>
+    <t>Prototype 3 [ Tags ]</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -513,17 +524,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" customWidth="1"/>
+    <col min="1" max="1" width="58.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
@@ -553,7 +564,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -562,7 +573,7 @@
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,10 +587,10 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -596,7 +607,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -630,19 +641,19 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -657,19 +668,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106BECBB-8D93-4A3B-AAAE-E4192AD3BAB2}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -741,7 +751,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,7 +762,7 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
@@ -769,7 +779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -785,13 +795,19 @@
       <c r="E17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -810,8 +826,12 @@
       <c r="F21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f>AVERAGE(B21:F21)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -830,8 +850,12 @@
       <c r="F22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" ref="G22:G23" si="0">AVERAGE(B22:F22)</f>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -850,11 +874,15 @@
       <c r="F23">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -871,21 +899,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45323CDF-F889-4C6F-9670-4C878856AA6C}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
@@ -902,29 +931,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -933,10 +962,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -955,8 +987,12 @@
       <c r="F7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>AVERAGE(B7:F7)</f>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -975,8 +1011,12 @@
       <c r="F8">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" ref="G8:G9" si="0">AVERAGE(B8:F8)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -995,17 +1035,21 @@
       <c r="F9">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1013,7 +1057,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1021,7 +1065,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1029,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1039,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0454749A-2141-49B1-B678-977DE214E3EB}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1097,7 @@
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1070,17 +1114,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1098,7 +1142,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1117,10 +1166,14 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>AVERAGE(B8:F8)</f>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>